<commit_message>
New statistisc sheet: now the data come from python. No more excel formulas
New sheet 'Statistiche per azioni'
</commit_message>
<xml_diff>
--- a/Trading_statistics.xlsx
+++ b/Trading_statistics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniovasile/Documents/Didattica e formazione/trading/Antonio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E14BDE4-2134-0242-88EE-17821A4E70A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3892F4-7799-6741-9377-4AAB00A0F952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operazioni" sheetId="1" r:id="rId1"/>
     <sheet name="Statistiche" sheetId="2" r:id="rId2"/>
-    <sheet name="Statistica per azione" sheetId="3" r:id="rId3"/>
+    <sheet name="Statistica per azione" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Operazioni!$A$1:$A$21</definedName>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="64">
   <si>
     <t>AZIONE</t>
   </si>
@@ -123,6 +123,9 @@
     <t>NET INCOME</t>
   </si>
   <si>
+    <t>-5.87$</t>
+  </si>
+  <si>
     <t>DAY START</t>
   </si>
   <si>
@@ -141,6 +144,9 @@
     <t>BATTING AVERAGE [%]</t>
   </si>
   <si>
+    <t>43.04%</t>
+  </si>
+  <si>
     <t>BEST DAY</t>
   </si>
   <si>
@@ -150,21 +156,36 @@
     <t>WIN</t>
   </si>
   <si>
+    <t>75.12$</t>
+  </si>
+  <si>
     <t>WORST DAY</t>
   </si>
   <si>
     <t>LOSS</t>
   </si>
   <si>
+    <t>-80.99$</t>
+  </si>
+  <si>
     <t>AVERAGE WIN</t>
   </si>
   <si>
+    <t>2.21$</t>
+  </si>
+  <si>
     <t>AVERAGE LOSS</t>
   </si>
   <si>
+    <t>-1.8$</t>
+  </si>
+  <si>
     <t>WIN/LOSS</t>
   </si>
   <si>
+    <t>1.23$</t>
+  </si>
+  <si>
     <t>Bilancio ultima giornata</t>
   </si>
   <si>
@@ -174,7 +195,37 @@
     <t>TOTAL AMOUNT</t>
   </si>
   <si>
+    <t>13.04$</t>
+  </si>
+  <si>
+    <t>53.85%</t>
+  </si>
+  <si>
+    <t>22.97$</t>
+  </si>
+  <si>
+    <t>-9.93$</t>
+  </si>
+  <si>
+    <t>3.28$</t>
+  </si>
+  <si>
+    <t>-1.66$</t>
+  </si>
+  <si>
+    <t>1.33$</t>
+  </si>
+  <si>
     <t>Bilancio Data:</t>
+  </si>
+  <si>
+    <t>NUMERO TRADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RISULTATO MEDIO </t>
+  </si>
+  <si>
+    <t>RISULTATO TOTALE</t>
   </si>
 </sst>
 </file>
@@ -279,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -289,100 +340,38 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -788,9 +777,9 @@
   </sheetPr>
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
+    <sheetView zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,7 +788,7 @@
     <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.1640625" customWidth="1"/>
     <col min="15" max="15" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -821,10 +810,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
-        <f>MAX(B:B)</f>
-        <v>44540</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1992,41 +1978,41 @@
   </sheetData>
   <autoFilter ref="A1:A21" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="D22:D1048576 D11:D17 D2:D8">
-    <cfRule type="cellIs" dxfId="14" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="38" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="13" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="37" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:D21">
-    <cfRule type="cellIs" dxfId="12" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D19">
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D71">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2038,10 +2024,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView topLeftCell="B4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I25" sqref="I25:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2054,520 +2040,468 @@
     <row r="2" spans="2:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="N4" s="11" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="N4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="11">
-        <f>MAX(Operazioni!D:D)</f>
-        <v>9.48</v>
-      </c>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="11">
-        <f>COUNTIF(Operazioni!D:D,"&lt;999999999999")</f>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="9">
         <v>79</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="11">
-        <f>MIN(Operazioni!D:D)</f>
-        <v>-5.75</v>
-      </c>
+      <c r="O5" s="9"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="8">
-        <f>SUM(Operazioni!D:D)</f>
-        <v>-5.8699999999999983</v>
-      </c>
-      <c r="N6" s="11" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="6">
-        <f>MIN(Operazioni!B:B)</f>
-        <v>44536</v>
-      </c>
+      <c r="N6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="6"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
+      <c r="B7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="5">
-        <f>COUNTIF(Operazioni!D:D,"&gt;0")</f>
         <v>34</v>
       </c>
-      <c r="N7" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" s="6">
-        <f>MAX(Operazioni!B:B)</f>
-        <v>44540</v>
-      </c>
+      <c r="N7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
+      <c r="B8" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="4">
-        <f>COUNTIF(Operazioni!D:D,"&lt;0")</f>
         <v>45</v>
       </c>
-      <c r="N8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="O8" s="8">
-        <f>E6/E5</f>
-        <v>-7.4303797468354416E-2</v>
-      </c>
+      <c r="N8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="8"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="11">
-        <f>(E7/E5)*100</f>
-        <v>43.037974683544306</v>
-      </c>
-      <c r="N9" s="11" t="s">
+      <c r="B9" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="13" t="s">
         <v>36</v>
       </c>
+      <c r="N9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="9">
-        <f>SUMIF(Operazioni!D:D,"&gt;0")</f>
-        <v>75.119999999999976</v>
-      </c>
-      <c r="N10" s="11" t="s">
+      <c r="B10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="O10" s="11" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="10">
-        <f>SUMIF(Operazioni!D:D,"&lt;0") * -1</f>
-        <v>80.990000000000009</v>
+      <c r="B11" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="9">
-        <f>E10/E7</f>
-        <v>2.2094117647058815</v>
+      <c r="B12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="10">
-        <f>E11/E8</f>
-        <v>1.7997777777777779</v>
+      <c r="B13" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="11">
-        <f>E12/(E13)</f>
-        <v>1.2276025362608305</v>
+      <c r="B14" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="6">
         <f>Operazioni!E1</f>
-        <v>44540</v>
-      </c>
-      <c r="I19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="18"/>
+      <c r="K19" s="7">
+        <v>44536</v>
+      </c>
+      <c r="L19" s="7">
+        <v>44543</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="13">
+        <v>13</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="5">
+        <v>7</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="14">
+        <v>6</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25" s="17"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" s="17"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="7">
-        <v>44536</v>
-      </c>
-      <c r="L19" s="7">
-        <v>44538</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="18" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="17"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="17"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="7">
+        <v>44540</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="11">
-        <f>COUNTIF(Operazioni!B:B,Operazioni!E1)</f>
+      <c r="C35" s="17"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="13">
         <v>13</v>
       </c>
-      <c r="I20" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="8">
-        <f>SUMIF(Operazioni!B:B,Operazioni!E1,Operazioni!D:D)</f>
-        <v>13.04</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="5">
-        <f>COUNTIFS(Operazioni!B:B,Operazioni!E1,Operazioni!D:D,"&gt;0")</f>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="4">
         <v>7</v>
       </c>
-      <c r="I22" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="4">
-        <f>COUNTIFS(Operazioni!B:B,Operazioni!E1,Operazioni!D:D,"&lt;0")</f>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="12">
         <v>6</v>
       </c>
-      <c r="I23" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="11">
-        <f>(E22/E20)*100</f>
-        <v>53.846153846153847</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="9">
-        <f>SUMIFS(Operazioni!D:D,Operazioni!B:B,Operazioni!E1,Operazioni!D:D,"&gt;0")</f>
-        <v>22.97</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="18" t="s">
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="10">
-        <f>SUMIFS(Operazioni!D:D,Operazioni!B:B,Operazioni!E1,Operazioni!D:D,"&lt;0") *-1</f>
-        <v>9.93</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="9">
-        <f>E25/E22</f>
-        <v>3.2814285714285711</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="10">
-        <f>E26/E23</f>
-        <v>1.655</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="18" t="s">
+      <c r="C40" s="17"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="11">
-        <f>E27/(E28)</f>
-        <v>1.9827362969356925</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="J29" s="19"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="21" t="s">
+      <c r="C41" s="17"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="7">
-        <v>44538</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="12">
-        <f>COUNTIF(Operazioni!B:B,E35)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="13">
-        <f>SUMIF(Operazioni!B:B,E35,Operazioni!D:D)</f>
-        <v>-22.2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="14">
-        <f>COUNTIFS(Operazioni!B:B,E35,Operazioni!D:D,"&gt;0")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="15">
-        <f>COUNTIFS(Operazioni!B:B,E35,Operazioni!D:D,"&lt;0")</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="12">
-        <f>(E38/E36)*100</f>
-        <v>35.294117647058826</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="16">
-        <f>SUMIFS(Operazioni!D:D,Operazioni!B:B,E35,Operazioni!D:D,"&gt;0")</f>
-        <v>4.79</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="17">
-        <f>SUMIFS(Operazioni!D:D,Operazioni!B:B,E35,Operazioni!D:D,"&lt;0") *-1</f>
-        <v>26.990000000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="16">
-        <f>E41/E38</f>
-        <v>0.79833333333333334</v>
+      <c r="C43" s="17"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="17">
-        <f>E42/E39</f>
-        <v>2.4536363636363636</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="12">
-        <f>E43/(E44)</f>
-        <v>0.32536742003211067</v>
+      <c r="B44" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B36:D36"/>
@@ -2578,63 +2512,68 @@
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="I20:K20"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Foglio3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="32.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Eliminate the excel command to calculate the last day.
</commit_message>
<xml_diff>
--- a/Trading_statistics.xlsx
+++ b/Trading_statistics.xlsx
@@ -8,28 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniovasile/Documents/Didattica e formazione/trading/Antonio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3892F4-7799-6741-9377-4AAB00A0F952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA798A7-CE9F-8645-BF2F-BD52BE1D0A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operazioni" sheetId="1" r:id="rId1"/>
     <sheet name="Statistiche" sheetId="2" r:id="rId2"/>
-    <sheet name="Statistica per azione" sheetId="4" r:id="rId3"/>
+    <sheet name="Statistica per azione" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Operazioni!$A$1:$A$21</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -2026,8 +2017,8 @@
   <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25:K25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2186,8 +2177,7 @@
       <c r="C19" s="17"/>
       <c r="D19" s="18"/>
       <c r="E19" s="6">
-        <f>Operazioni!E1</f>
-        <v>0</v>
+        <v>44540</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>51</v>
@@ -2543,11 +2533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Foglio3"/>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Added run.py to run all the scripts. - inserted TODO in StatisticsPerShares - Inserted template in NewOperations sheet.
</commit_message>
<xml_diff>
--- a/Trading_statistics.xlsx
+++ b/Trading_statistics.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Statistica_per_azione" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Operazioni'!$A$1:$A$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Operazioni'!$A$1</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -19,8 +19,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -137,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -170,13 +171,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -586,11 +588,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -634,206 +636,194 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAPL</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>44540</v>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B2" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C2" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D2" t="n">
-        <v>3.17</v>
-      </c>
-      <c r="E2" s="1" t="n"/>
+        <v>0.31</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AAPL</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>44540</v>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B3" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C3" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D3" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="E3" s="1" t="n"/>
+        <v>0.08</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MSFT</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>44540</v>
+          <t>NFLX</t>
+        </is>
+      </c>
+      <c r="B4" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C4" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.45</v>
-      </c>
-      <c r="E4" s="1" t="n"/>
+        <v>-0.84</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>INTC</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>44540</v>
+          <t>DIS</t>
+        </is>
+      </c>
+      <c r="B5" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C5" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.42</v>
-      </c>
-      <c r="E5" s="1" t="n"/>
+        <v>0.26</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NFLX</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>44540</v>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B6" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C6" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.74</v>
-      </c>
-      <c r="E6" s="1" t="n"/>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>JNJ</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>44540</v>
+          <t>VIR</t>
+        </is>
+      </c>
+      <c r="B7" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C7" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D7" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="E7" s="1" t="n"/>
+        <v>-3.18</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MU</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>44540</v>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="B8" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C8" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.65</v>
-      </c>
-      <c r="E8" s="1" t="n"/>
+        <v>2.82</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MRNA</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>44540</v>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B9" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C9" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.1</v>
-      </c>
-      <c r="E9" s="1" t="n"/>
+        <v>1.83</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MSFT</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>44540</v>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B10" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C10" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D10" t="n">
-        <v>6.61</v>
-      </c>
-      <c r="E10" s="1" t="n"/>
+        <v>2.87</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MRNA</t>
-        </is>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>44540</v>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B11" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C11" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D11" t="n">
-        <v>4.63</v>
-      </c>
-      <c r="E11" s="1" t="n"/>
+        <v>0.26</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AAPL</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>44540</v>
+          <t>MRNA</t>
+        </is>
+      </c>
+      <c r="B12" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C12" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D12" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="E12" s="1" t="n"/>
+        <v>-3.43</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NVAX</t>
-        </is>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>44540</v>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B13" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C13" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D13" t="n">
-        <v>6.11</v>
-      </c>
-      <c r="E13" s="1" t="n"/>
+        <v>3.85</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -841,521 +831,514 @@
           <t>NVDA</t>
         </is>
       </c>
-      <c r="B14" s="1" t="n">
-        <v>44540</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>44540</v>
+      <c r="B14" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C14" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D14" t="n">
-        <v>-2.57</v>
-      </c>
-      <c r="E14" s="1" t="n"/>
+        <v>3.58</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PFE</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>44539</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>44539</v>
+          <t>MRNA</t>
+        </is>
+      </c>
+      <c r="B15" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C15" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D15" t="n">
-        <v>-3.25</v>
-      </c>
-      <c r="E15" s="1" t="n"/>
+        <v>4.3</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>JNJ</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>44539</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>44539</v>
+          <t>BNTX</t>
+        </is>
+      </c>
+      <c r="B16" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C16" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D16" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="E16" s="1" t="n"/>
+        <v>-5.15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>FB</t>
-        </is>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>44539</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>44539</v>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B17" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C17" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.04</v>
-      </c>
-      <c r="E17" s="1" t="n"/>
+        <v>-0.89</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NFLX</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>44539</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>44539</v>
+          <t>NVAX</t>
+        </is>
+      </c>
+      <c r="B18" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C18" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.18</v>
-      </c>
-      <c r="E18" s="1" t="n"/>
+        <v>-3.61</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DIS</t>
-        </is>
-      </c>
-      <c r="B19" s="1" t="n">
-        <v>44539</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>44539</v>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="B19" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C19" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.8100000000000001</v>
-      </c>
-      <c r="E19" s="1" t="n"/>
+        <v>-1.99</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>VIR</t>
-        </is>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>44539</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>44539</v>
+          <t>MRNA</t>
+        </is>
+      </c>
+      <c r="B20" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C20" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D20" t="n">
-        <v>1.68</v>
-      </c>
-      <c r="E20" s="1" t="n"/>
+        <v>-2.2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="B21" s="1" t="n">
-        <v>44539</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>44539</v>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="B21" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C21" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D21" t="n">
-        <v>-1.38</v>
-      </c>
-      <c r="E21" s="1" t="n"/>
+        <v>4.96</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AMZN</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>44539</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>44539</v>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="B22" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C22" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D22" t="n">
-        <v>-1.27</v>
-      </c>
-      <c r="E22" s="1" t="n"/>
+        <v>-3.07</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>FB</t>
-        </is>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>44538</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>44538</v>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B23" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C23" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.96</v>
-      </c>
-      <c r="E23" s="1" t="n"/>
+        <v>-4.9</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>INTC</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>44538</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>44538</v>
+          <t>MRNA</t>
+        </is>
+      </c>
+      <c r="B24" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C24" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D24" t="n">
-        <v>1.45</v>
-      </c>
-      <c r="E24" s="1" t="n"/>
+        <v>2.41</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>JNJ</t>
-        </is>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>44538</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>44538</v>
+          <t>NVAX</t>
+        </is>
+      </c>
+      <c r="B25" s="21" t="n">
+        <v>44543</v>
+      </c>
+      <c r="C25" s="21" t="n">
+        <v>44543</v>
       </c>
       <c r="D25" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="E25" s="1" t="n"/>
+        <v>-4.17</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B26" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.62</v>
+        <v>3.17</v>
       </c>
       <c r="E26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B27" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D27" t="n">
-        <v>0.13</v>
+        <v>0.37</v>
       </c>
       <c r="E27" s="1" t="n"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MRNA</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B28" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D28" t="n">
-        <v>-1.79</v>
+        <v>-1.45</v>
       </c>
       <c r="E28" s="1" t="n"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B29" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D29" t="n">
-        <v>0.88</v>
+        <v>-1.42</v>
       </c>
       <c r="E29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>MRNA</t>
+          <t>NFLX</t>
         </is>
       </c>
       <c r="B30" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D30" t="n">
-        <v>-4.6</v>
+        <v>-0.74</v>
       </c>
       <c r="E30" s="1" t="n"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>VIR</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B31" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D31" t="n">
-        <v>-3.05</v>
+        <v>1.97</v>
       </c>
       <c r="E31" s="1" t="n"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GOOG</t>
+          <t>MU</t>
         </is>
       </c>
       <c r="B32" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D32" t="n">
-        <v>-1.7</v>
+        <v>-1.65</v>
       </c>
       <c r="E32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MU</t>
+          <t>MRNA</t>
         </is>
       </c>
       <c r="B33" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D33" t="n">
-        <v>1.31</v>
+        <v>-2.1</v>
       </c>
       <c r="E33" s="1" t="n"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B34" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.73</v>
+        <v>6.61</v>
       </c>
       <c r="E34" s="1" t="n"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>AMZN</t>
+          <t>MRNA</t>
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D35" t="n">
-        <v>-1.22</v>
+        <v>4.63</v>
       </c>
       <c r="E35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>NVAX</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B36" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D36" t="n">
-        <v>-5.75</v>
+        <v>0.11</v>
       </c>
       <c r="E36" s="1" t="n"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>GOOG</t>
+          <t>NVAX</t>
         </is>
       </c>
       <c r="B37" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D37" t="n">
-        <v>0.19</v>
+        <v>6.11</v>
       </c>
       <c r="E37" s="1" t="n"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>TSLA</t>
+          <t>NVDA</t>
         </is>
       </c>
       <c r="B38" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44538</v>
+        <v>44540</v>
       </c>
       <c r="D38" t="n">
-        <v>-1.21</v>
+        <v>-2.57</v>
       </c>
       <c r="E38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>NVAX</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B39" s="1" t="n">
-        <v>44538</v>
+        <v>44539</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44538</v>
+        <v>44539</v>
       </c>
       <c r="D39" t="n">
-        <v>-5.36</v>
+        <v>-3.25</v>
       </c>
       <c r="E39" s="1" t="n"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>LIT</t>
-        </is>
-      </c>
-      <c r="B40" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C40" s="3" t="n">
-        <v>44537</v>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>44539</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>44539</v>
       </c>
       <c r="D40" t="n">
-        <v>-2.19</v>
-      </c>
+        <v>0.88</v>
+      </c>
+      <c r="E40" s="1" t="n"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>JNJ</t>
-        </is>
-      </c>
-      <c r="B41" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C41" s="3" t="n">
-        <v>44537</v>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>44539</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>44539</v>
       </c>
       <c r="D41" t="n">
-        <v>0.64</v>
-      </c>
+        <v>-1.04</v>
+      </c>
+      <c r="E41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>MSFT</t>
-        </is>
-      </c>
-      <c r="B42" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C42" s="3" t="n">
-        <v>44537</v>
+          <t>NFLX</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>44539</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>44539</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.92</v>
-      </c>
+        <v>-1.18</v>
+      </c>
+      <c r="E42" s="1" t="n"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="B43" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C43" s="3" t="n">
-        <v>44537</v>
+          <t>DIS</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>44539</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>44539</v>
       </c>
       <c r="D43" t="n">
-        <v>-1.14</v>
-      </c>
+        <v>-0.8100000000000001</v>
+      </c>
+      <c r="E43" s="1" t="n"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>INTC</t>
-        </is>
-      </c>
-      <c r="B44" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C44" s="3" t="n">
-        <v>44537</v>
+          <t>VIR</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>44539</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>44539</v>
       </c>
       <c r="D44" t="n">
-        <v>-2.18</v>
-      </c>
+        <v>1.68</v>
+      </c>
+      <c r="E44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1363,127 +1346,135 @@
           <t>NVDA</t>
         </is>
       </c>
-      <c r="B45" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C45" s="3" t="n">
-        <v>44537</v>
+      <c r="B45" s="1" t="n">
+        <v>44539</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>44539</v>
       </c>
       <c r="D45" t="n">
-        <v>2.12</v>
-      </c>
+        <v>-1.38</v>
+      </c>
+      <c r="E45" s="1" t="n"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>JNJ</t>
-        </is>
-      </c>
-      <c r="B46" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C46" s="3" t="n">
-        <v>44537</v>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>44539</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>44539</v>
       </c>
       <c r="D46" t="n">
-        <v>0.36</v>
-      </c>
+        <v>-1.27</v>
+      </c>
+      <c r="E46" s="1" t="n"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>DIS</t>
-        </is>
-      </c>
-      <c r="B47" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C47" s="3" t="n">
-        <v>44537</v>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D47" t="n">
-        <v>-1.39</v>
-      </c>
+        <v>-0.96</v>
+      </c>
+      <c r="E47" s="1" t="n"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="B48" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C48" s="3" t="n">
-        <v>44537</v>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D48" t="n">
-        <v>0.59</v>
-      </c>
+        <v>1.45</v>
+      </c>
+      <c r="E48" s="1" t="n"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="B49" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C49" s="3" t="n">
-        <v>44537</v>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D49" t="n">
-        <v>0.76</v>
-      </c>
+        <v>0.83</v>
+      </c>
+      <c r="E49" s="1" t="n"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="B50" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C50" s="3" t="n">
-        <v>44537</v>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.21</v>
-      </c>
+        <v>-0.62</v>
+      </c>
+      <c r="E50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>AMZN</t>
-        </is>
-      </c>
-      <c r="B51" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C51" s="3" t="n">
-        <v>44537</v>
+          <t>DIS</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D51" t="n">
-        <v>0.12</v>
-      </c>
+        <v>0.13</v>
+      </c>
+      <c r="E51" s="1" t="n"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>TSLA</t>
-        </is>
-      </c>
-      <c r="B52" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C52" s="3" t="n">
-        <v>44537</v>
+          <t>MRNA</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D52" t="n">
-        <v>1.39</v>
-      </c>
+        <v>-1.79</v>
+      </c>
+      <c r="E52" s="1" t="n"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1491,111 +1482,118 @@
           <t>MSFT</t>
         </is>
       </c>
-      <c r="B53" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C53" s="3" t="n">
-        <v>44537</v>
+      <c r="B53" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D53" t="n">
-        <v>0.37</v>
-      </c>
+        <v>0.88</v>
+      </c>
+      <c r="E53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>NFLX</t>
-        </is>
-      </c>
-      <c r="B54" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C54" s="3" t="n">
-        <v>44537</v>
+          <t>MRNA</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D54" t="n">
-        <v>1.14</v>
-      </c>
+        <v>-4.6</v>
+      </c>
+      <c r="E54" s="1" t="n"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>INTC</t>
-        </is>
-      </c>
-      <c r="B55" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C55" s="3" t="n">
-        <v>44537</v>
+          <t>VIR</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.07000000000000001</v>
-      </c>
+        <v>-3.05</v>
+      </c>
+      <c r="E55" s="1" t="n"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>PFE</t>
-        </is>
-      </c>
-      <c r="B56" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C56" s="3" t="n">
-        <v>44537</v>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D56" t="n">
-        <v>0.42</v>
-      </c>
+        <v>-1.7</v>
+      </c>
+      <c r="E56" s="1" t="n"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="B57" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C57" s="3" t="n">
-        <v>44537</v>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D57" t="n">
-        <v>0.06</v>
-      </c>
+        <v>1.31</v>
+      </c>
+      <c r="E57" s="1" t="n"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>AMZN</t>
-        </is>
-      </c>
-      <c r="B58" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C58" s="3" t="n">
-        <v>44537</v>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D58" t="n">
-        <v>-2.45</v>
-      </c>
+        <v>-0.73</v>
+      </c>
+      <c r="E58" s="1" t="n"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>NVAX</t>
-        </is>
-      </c>
-      <c r="B59" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C59" s="3" t="n">
-        <v>44537</v>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.77</v>
-      </c>
+        <v>-1.22</v>
+      </c>
+      <c r="E59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1603,94 +1601,98 @@
           <t>NVAX</t>
         </is>
       </c>
-      <c r="B60" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C60" s="3" t="n">
-        <v>44537</v>
+      <c r="B60" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D60" t="n">
-        <v>-1.17</v>
-      </c>
+        <v>-5.75</v>
+      </c>
+      <c r="E60" s="1" t="n"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="B61" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C61" s="3" t="n">
-        <v>44537</v>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D61" t="n">
-        <v>4.4</v>
-      </c>
+        <v>0.19</v>
+      </c>
+      <c r="E61" s="1" t="n"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MU</t>
-        </is>
-      </c>
-      <c r="B62" s="3" t="n">
-        <v>44537</v>
-      </c>
-      <c r="C62" s="3" t="n">
-        <v>44537</v>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>44538</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D62" t="n">
-        <v>3.3</v>
-      </c>
+        <v>-1.21</v>
+      </c>
+      <c r="E62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>NVAX</t>
         </is>
       </c>
       <c r="B63" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C63" s="3" t="n">
-        <v>44537</v>
+        <v>44538</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>44538</v>
       </c>
       <c r="D63" t="n">
-        <v>9.48</v>
-      </c>
+        <v>-5.36</v>
+      </c>
+      <c r="E63" s="1" t="n"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>GOOG</t>
-        </is>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>44536</v>
+          <t>LIT</t>
+        </is>
+      </c>
+      <c r="B64" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="C64" s="3" t="n">
         <v>44537</v>
       </c>
       <c r="D64" t="n">
-        <v>9.140000000000001</v>
+        <v>-2.19</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="B65" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>44536</v>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B65" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C65" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D65" t="n">
-        <v>-1.82</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="66">
@@ -1699,273 +1701,657 @@
           <t>MSFT</t>
         </is>
       </c>
-      <c r="B66" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C66" s="1" t="n">
-        <v>44536</v>
+      <c r="B66" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C66" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.85</v>
+        <v>-0.92</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>PHG</t>
-        </is>
-      </c>
-      <c r="B67" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>44536</v>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="B67" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C67" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D67" t="n">
-        <v>-2.7</v>
+        <v>-1.14</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="B68" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C68" s="1" t="n">
-        <v>44536</v>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B68" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C68" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.9399999999999999</v>
+        <v>-2.18</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>TSLA</t>
-        </is>
-      </c>
-      <c r="B69" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C69" s="1" t="n">
-        <v>44536</v>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B69" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C69" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D69" t="n">
-        <v>5.75</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>AMZN</t>
-        </is>
-      </c>
-      <c r="B70" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>44536</v>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B70" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C70" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D70" t="n">
-        <v>1.47</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>INTC</t>
-        </is>
-      </c>
-      <c r="B71" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C71" s="1" t="n">
-        <v>44536</v>
+          <t>DIS</t>
+        </is>
+      </c>
+      <c r="B71" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C71" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D71" t="n">
-        <v>1.82</v>
+        <v>-1.39</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>VIR</t>
-        </is>
-      </c>
-      <c r="B72" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>44536</v>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B72" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C72" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D72" t="n">
-        <v>-4.2</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DIS</t>
-        </is>
-      </c>
-      <c r="B73" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>44536</v>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="B73" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C73" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D73" t="n">
-        <v>1.47</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MSFT</t>
-        </is>
-      </c>
-      <c r="B74" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>44536</v>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="B74" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C74" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D74" t="n">
-        <v>-0.44</v>
+        <v>-1.21</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="B75" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>44536</v>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B75" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C75" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.31</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="inlineStr">
-        <is>
-          <t>MSFT</t>
-        </is>
-      </c>
-      <c r="B76" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C76" s="1" t="n">
-        <v>44536</v>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B76" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C76" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D76" t="n">
-        <v>-0.24</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>PFE</t>
-        </is>
-      </c>
-      <c r="B77" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C77" s="1" t="n">
-        <v>44536</v>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B77" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C77" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D77" t="n">
-        <v>-3</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>FB</t>
-        </is>
-      </c>
-      <c r="B78" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C78" s="1" t="n">
-        <v>44536</v>
+          <t>NFLX</t>
+        </is>
+      </c>
+      <c r="B78" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C78" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D78" t="n">
-        <v>-1.18</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>NVAX</t>
-        </is>
-      </c>
-      <c r="B79" s="1" t="n">
-        <v>44536</v>
-      </c>
-      <c r="C79" s="1" t="n">
-        <v>44536</v>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B79" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C79" s="3" t="n">
+        <v>44537</v>
       </c>
       <c r="D79" t="n">
-        <v>-5.59</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="B80" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C80" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B81" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C81" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B82" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C82" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D82" t="n">
+        <v>-2.45</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>NVAX</t>
+        </is>
+      </c>
+      <c r="B83" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C83" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D83" t="n">
+        <v>-0.77</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>NVAX</t>
+        </is>
+      </c>
+      <c r="B84" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C84" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D84" t="n">
+        <v>-1.17</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B85" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C85" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D85" t="n">
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="B86" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="C86" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D86" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C87" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D87" t="n">
+        <v>9.48</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C88" s="3" t="n">
+        <v>44537</v>
+      </c>
+      <c r="D88" t="n">
+        <v>9.140000000000001</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D89" t="n">
+        <v>-1.82</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B90" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D90" t="n">
+        <v>-0.85</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>PHG</t>
+        </is>
+      </c>
+      <c r="B91" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C91" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D91" t="n">
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="B92" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C92" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D92" t="n">
+        <v>-0.9399999999999999</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C93" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D93" t="n">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B94" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B95" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D95" t="n">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>VIR</t>
+        </is>
+      </c>
+      <c r="B96" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D96" t="n">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>DIS</t>
+        </is>
+      </c>
+      <c r="B97" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B98" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D98" t="n">
+        <v>-0.44</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B99" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D99" t="n">
+        <v>-0.31</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B100" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D100" t="n">
+        <v>-0.24</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="B101" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D101" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="B80" s="1" t="n">
+      <c r="B102" s="1" t="n">
         <v>44536</v>
       </c>
-      <c r="C80" s="1" t="n">
+      <c r="C102" s="1" t="n">
         <v>44536</v>
       </c>
-      <c r="D80" t="n">
+      <c r="D102" t="n">
+        <v>-1.18</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>NVAX</t>
+        </is>
+      </c>
+      <c r="B103" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C103" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D103" t="n">
+        <v>-5.59</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="B104" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="C104" s="1" t="n">
+        <v>44536</v>
+      </c>
+      <c r="D104" t="n">
         <v>-0.38</v>
       </c>
     </row>
-    <row r="81">
-      <c r="B81" s="1" t="n"/>
-    </row>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88">
-      <c r="B88" s="1" t="n"/>
-      <c r="C88" s="1" t="n"/>
-    </row>
-    <row r="89">
-      <c r="B89" s="1" t="n"/>
-      <c r="C89" s="1" t="n"/>
-    </row>
-    <row r="90">
-      <c r="B90" s="1" t="n"/>
-      <c r="C90" s="3" t="n"/>
-    </row>
-    <row r="91">
-      <c r="B91" s="1" t="n"/>
-      <c r="C91" s="3" t="n"/>
+    <row r="105">
+      <c r="B105" s="1" t="n"/>
+    </row>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112">
+      <c r="B112" s="1" t="n"/>
+      <c r="C112" s="1" t="n"/>
+    </row>
+    <row r="113">
+      <c r="B113" s="1" t="n"/>
+      <c r="C113" s="1" t="n"/>
+    </row>
+    <row r="114">
+      <c r="B114" s="1" t="n"/>
+      <c r="C114" s="3" t="n"/>
+    </row>
+    <row r="115">
+      <c r="B115" s="1" t="n"/>
+      <c r="C115" s="3" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A3"/>
-  <conditionalFormatting sqref="D4:D1048576">
+  <autoFilter ref="A1"/>
+  <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="cellIs" priority="38" operator="lessThan" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D53">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="22" operator="greaterThan" dxfId="1">
       <formula>0</formula>
     </cfRule>
@@ -1986,8 +2372,8 @@
   </sheetPr>
   <dimension ref="B4:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="B4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2000,7 +2386,7 @@
     <row r="2" hidden="1"/>
     <row r="3" hidden="1"/>
     <row r="4">
-      <c r="B4" s="17" t="inlineStr">
+      <c r="B4" s="20" t="inlineStr">
         <is>
           <t>Bilancio totale</t>
         </is>
@@ -2016,7 +2402,7 @@
       <c r="O4" s="9" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="20" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>Totale operazioni</t>
         </is>
@@ -2024,7 +2410,7 @@
       <c r="C5" s="18" t="n"/>
       <c r="D5" s="19" t="n"/>
       <c r="E5" s="9" t="n">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="N5" s="9" t="inlineStr">
         <is>
@@ -2034,7 +2420,7 @@
       <c r="O5" s="9" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="20" t="inlineStr">
+      <c r="B6" s="17" t="inlineStr">
         <is>
           <t>NET INCOME</t>
         </is>
@@ -2043,7 +2429,7 @@
       <c r="D6" s="19" t="n"/>
       <c r="E6" s="15" t="inlineStr">
         <is>
-          <t>-5.87$</t>
+          <t>-11.71$</t>
         </is>
       </c>
       <c r="N6" s="9" t="inlineStr">
@@ -2054,7 +2440,7 @@
       <c r="O6" s="6" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="20" t="inlineStr">
+      <c r="B7" s="17" t="inlineStr">
         <is>
           <t>OPERAZIONI IN GUADAGNO</t>
         </is>
@@ -2062,7 +2448,7 @@
       <c r="C7" s="18" t="n"/>
       <c r="D7" s="19" t="n"/>
       <c r="E7" s="5" t="n">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="N7" s="9" t="inlineStr">
         <is>
@@ -2072,7 +2458,7 @@
       <c r="O7" s="6" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="20" t="inlineStr">
+      <c r="B8" s="17" t="inlineStr">
         <is>
           <t>OPERAZIONI IN PERDITA</t>
         </is>
@@ -2080,7 +2466,7 @@
       <c r="C8" s="18" t="n"/>
       <c r="D8" s="19" t="n"/>
       <c r="E8" s="4" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="N8" s="9" t="inlineStr">
         <is>
@@ -2090,7 +2476,7 @@
       <c r="O8" s="8" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" s="20" t="inlineStr">
+      <c r="B9" s="17" t="inlineStr">
         <is>
           <t>BATTING AVERAGE [%]</t>
         </is>
@@ -2099,7 +2485,7 @@
       <c r="D9" s="19" t="n"/>
       <c r="E9" s="13" t="inlineStr">
         <is>
-          <t>43.04%</t>
+          <t>45.63%</t>
         </is>
       </c>
       <c r="N9" s="9" t="inlineStr">
@@ -2114,7 +2500,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="20" t="inlineStr">
+      <c r="B10" s="17" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
@@ -2123,7 +2509,7 @@
       <c r="D10" s="19" t="n"/>
       <c r="E10" s="10" t="inlineStr">
         <is>
-          <t>75.12$</t>
+          <t>102.71$</t>
         </is>
       </c>
       <c r="N10" s="9" t="inlineStr">
@@ -2138,7 +2524,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="20" t="inlineStr">
+      <c r="B11" s="17" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
@@ -2147,12 +2533,12 @@
       <c r="D11" s="19" t="n"/>
       <c r="E11" s="11" t="inlineStr">
         <is>
-          <t>-80.99$</t>
+          <t>-114.42$</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="20" t="inlineStr">
+      <c r="B12" s="17" t="inlineStr">
         <is>
           <t>AVERAGE WIN</t>
         </is>
@@ -2161,12 +2547,12 @@
       <c r="D12" s="19" t="n"/>
       <c r="E12" s="10" t="inlineStr">
         <is>
-          <t>2.21$</t>
+          <t>2.19$</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="20" t="inlineStr">
+      <c r="B13" s="17" t="inlineStr">
         <is>
           <t>AVERAGE LOSS</t>
         </is>
@@ -2175,12 +2561,12 @@
       <c r="D13" s="19" t="n"/>
       <c r="E13" s="11" t="inlineStr">
         <is>
-          <t>-1.8$</t>
+          <t>-2.04$</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="20" t="inlineStr">
+      <c r="B14" s="17" t="inlineStr">
         <is>
           <t>WIN/LOSS</t>
         </is>
@@ -2189,12 +2575,12 @@
       <c r="D14" s="19" t="n"/>
       <c r="E14" s="13" t="inlineStr">
         <is>
-          <t>1.23$</t>
+          <t>1.07$</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="17" t="inlineStr">
+      <c r="B19" s="20" t="inlineStr">
         <is>
           <t>Bilancio ultima giornata</t>
         </is>
@@ -2202,9 +2588,9 @@
       <c r="C19" s="18" t="n"/>
       <c r="D19" s="19" t="n"/>
       <c r="E19" s="6" t="n">
-        <v>44540</v>
-      </c>
-      <c r="I19" s="17" t="inlineStr">
+        <v>44543</v>
+      </c>
+      <c r="I19" s="20" t="inlineStr">
         <is>
           <t>Bilancio Intervallo:</t>
         </is>
@@ -2218,7 +2604,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="20" t="inlineStr">
+      <c r="B20" s="17" t="inlineStr">
         <is>
           <t>Totale operazioni</t>
         </is>
@@ -2226,9 +2612,9 @@
       <c r="C20" s="18" t="n"/>
       <c r="D20" s="19" t="n"/>
       <c r="E20" s="13" t="n">
-        <v>13</v>
-      </c>
-      <c r="I20" s="20" t="inlineStr">
+        <v>24</v>
+      </c>
+      <c r="I20" s="17" t="inlineStr">
         <is>
           <t>Totale operazioni</t>
         </is>
@@ -2236,11 +2622,11 @@
       <c r="J20" s="18" t="n"/>
       <c r="K20" s="19" t="n"/>
       <c r="L20" s="13" t="n">
-        <v>79</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="20" t="inlineStr">
+      <c r="B21" s="17" t="inlineStr">
         <is>
           <t>TOTAL AMOUNT</t>
         </is>
@@ -2249,10 +2635,10 @@
       <c r="D21" s="19" t="n"/>
       <c r="E21" s="15" t="inlineStr">
         <is>
-          <t>13.04$</t>
-        </is>
-      </c>
-      <c r="I21" s="20" t="inlineStr">
+          <t>-5.84$</t>
+        </is>
+      </c>
+      <c r="I21" s="17" t="inlineStr">
         <is>
           <t>TOTAL AMOUNT</t>
         </is>
@@ -2261,12 +2647,12 @@
       <c r="K21" s="19" t="n"/>
       <c r="L21" s="13" t="inlineStr">
         <is>
-          <t>-5.87$</t>
+          <t>-11.71$</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="20" t="inlineStr">
+      <c r="B22" s="17" t="inlineStr">
         <is>
           <t>OPERAZIONI IN GUADAGNO</t>
         </is>
@@ -2274,9 +2660,9 @@
       <c r="C22" s="18" t="n"/>
       <c r="D22" s="19" t="n"/>
       <c r="E22" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="I22" s="20" t="inlineStr">
+        <v>13</v>
+      </c>
+      <c r="I22" s="17" t="inlineStr">
         <is>
           <t>OPERAZIONI IN GUADAGNO</t>
         </is>
@@ -2284,11 +2670,11 @@
       <c r="J22" s="18" t="n"/>
       <c r="K22" s="19" t="n"/>
       <c r="L22" s="5" t="n">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="20" t="inlineStr">
+      <c r="B23" s="17" t="inlineStr">
         <is>
           <t>OPERAZIONI IN PERDITA</t>
         </is>
@@ -2296,9 +2682,9 @@
       <c r="C23" s="18" t="n"/>
       <c r="D23" s="19" t="n"/>
       <c r="E23" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="I23" s="20" t="inlineStr">
+        <v>11</v>
+      </c>
+      <c r="I23" s="17" t="inlineStr">
         <is>
           <t>OPERAZIONI IN PERDITA</t>
         </is>
@@ -2306,11 +2692,11 @@
       <c r="J23" s="18" t="n"/>
       <c r="K23" s="19" t="n"/>
       <c r="L23" s="14" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="20" t="inlineStr">
+      <c r="B24" s="17" t="inlineStr">
         <is>
           <t>BATTING AVERAGE [%]</t>
         </is>
@@ -2319,10 +2705,10 @@
       <c r="D24" s="19" t="n"/>
       <c r="E24" s="15" t="inlineStr">
         <is>
-          <t>53.85%</t>
-        </is>
-      </c>
-      <c r="I24" s="20" t="inlineStr">
+          <t>54.17%</t>
+        </is>
+      </c>
+      <c r="I24" s="17" t="inlineStr">
         <is>
           <t>BATTING AVERAGE [%]</t>
         </is>
@@ -2331,12 +2717,12 @@
       <c r="K24" s="19" t="n"/>
       <c r="L24" s="15" t="inlineStr">
         <is>
-          <t>43.04%</t>
+          <t>45.63%</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="20" t="inlineStr">
+      <c r="B25" s="17" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
@@ -2345,10 +2731,10 @@
       <c r="D25" s="19" t="n"/>
       <c r="E25" s="10" t="inlineStr">
         <is>
-          <t>22.97$</t>
-        </is>
-      </c>
-      <c r="I25" s="20" t="inlineStr">
+          <t>27.59$</t>
+        </is>
+      </c>
+      <c r="I25" s="17" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
@@ -2357,12 +2743,12 @@
       <c r="K25" s="19" t="n"/>
       <c r="L25" s="10" t="inlineStr">
         <is>
-          <t>75.12$</t>
+          <t>102.71$</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="20" t="inlineStr">
+      <c r="B26" s="17" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
@@ -2371,10 +2757,10 @@
       <c r="D26" s="19" t="n"/>
       <c r="E26" s="11" t="inlineStr">
         <is>
-          <t>-9.93$</t>
-        </is>
-      </c>
-      <c r="I26" s="20" t="inlineStr">
+          <t>-33.43$</t>
+        </is>
+      </c>
+      <c r="I26" s="17" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
@@ -2383,12 +2769,12 @@
       <c r="K26" s="19" t="n"/>
       <c r="L26" s="11" t="inlineStr">
         <is>
-          <t>-80.99$</t>
+          <t>-114.42$</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="20" t="inlineStr">
+      <c r="B27" s="17" t="inlineStr">
         <is>
           <t>AVERAGE WIN</t>
         </is>
@@ -2397,10 +2783,10 @@
       <c r="D27" s="19" t="n"/>
       <c r="E27" s="10" t="inlineStr">
         <is>
-          <t>3.28$</t>
-        </is>
-      </c>
-      <c r="I27" s="20" t="inlineStr">
+          <t>2.12$</t>
+        </is>
+      </c>
+      <c r="I27" s="17" t="inlineStr">
         <is>
           <t>AVERAGE WIN</t>
         </is>
@@ -2409,12 +2795,12 @@
       <c r="K27" s="19" t="n"/>
       <c r="L27" s="10" t="inlineStr">
         <is>
-          <t>2.21$</t>
+          <t>2.19$</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="20" t="inlineStr">
+      <c r="B28" s="17" t="inlineStr">
         <is>
           <t>AVERAGE LOSS</t>
         </is>
@@ -2423,10 +2809,10 @@
       <c r="D28" s="19" t="n"/>
       <c r="E28" s="14" t="inlineStr">
         <is>
-          <t>-1.66$</t>
-        </is>
-      </c>
-      <c r="I28" s="20" t="inlineStr">
+          <t>-3.04$</t>
+        </is>
+      </c>
+      <c r="I28" s="17" t="inlineStr">
         <is>
           <t>AVERAGE LOSS</t>
         </is>
@@ -2435,12 +2821,12 @@
       <c r="K28" s="19" t="n"/>
       <c r="L28" s="14" t="inlineStr">
         <is>
-          <t>-1.8$</t>
+          <t>-2.04$</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="20" t="inlineStr">
+      <c r="B29" s="17" t="inlineStr">
         <is>
           <t>WIN/LOSS</t>
         </is>
@@ -2449,10 +2835,10 @@
       <c r="D29" s="19" t="n"/>
       <c r="E29" s="15" t="inlineStr">
         <is>
-          <t>1.33$</t>
-        </is>
-      </c>
-      <c r="I29" s="20" t="inlineStr">
+          <t>0.72$</t>
+        </is>
+      </c>
+      <c r="I29" s="17" t="inlineStr">
         <is>
           <t>WIN/LOSS</t>
         </is>
@@ -2461,12 +2847,12 @@
       <c r="K29" s="19" t="n"/>
       <c r="L29" s="15" t="inlineStr">
         <is>
-          <t>1.23$</t>
+          <t>1.07$</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="17" t="inlineStr">
+      <c r="B34" s="20" t="inlineStr">
         <is>
           <t>Bilancio Data:</t>
         </is>
@@ -2478,7 +2864,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="20" t="inlineStr">
+      <c r="B35" s="17" t="inlineStr">
         <is>
           <t>Totale operazioni</t>
         </is>
@@ -2490,7 +2876,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="20" t="inlineStr">
+      <c r="B36" s="17" t="inlineStr">
         <is>
           <t>TOTAL AMOUNT</t>
         </is>
@@ -2504,7 +2890,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="B37" s="20" t="inlineStr">
+      <c r="B37" s="17" t="inlineStr">
         <is>
           <t>OPERAZIONI IN GUADAGNO</t>
         </is>
@@ -2516,7 +2902,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="20" t="inlineStr">
+      <c r="B38" s="17" t="inlineStr">
         <is>
           <t>OPERAZIONI IN PERDITA</t>
         </is>
@@ -2528,7 +2914,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="20" t="inlineStr">
+      <c r="B39" s="17" t="inlineStr">
         <is>
           <t>BATTING AVERAGE [%]</t>
         </is>
@@ -2542,7 +2928,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="20" t="inlineStr">
+      <c r="B40" s="17" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
@@ -2556,7 +2942,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="20" t="inlineStr">
+      <c r="B41" s="17" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
@@ -2570,7 +2956,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="20" t="inlineStr">
+      <c r="B42" s="17" t="inlineStr">
         <is>
           <t>AVERAGE WIN</t>
         </is>
@@ -2584,7 +2970,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="20" t="inlineStr">
+      <c r="B43" s="17" t="inlineStr">
         <is>
           <t>AVERAGE LOSS</t>
         </is>
@@ -2598,7 +2984,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="B44" s="20" t="inlineStr">
+      <c r="B44" s="17" t="inlineStr">
         <is>
           <t>WIN/LOSS</t>
         </is>
@@ -2607,34 +2993,18 @@
       <c r="D44" s="19" t="n"/>
       <c r="E44" s="15" t="inlineStr">
         <is>
-          <t>1.33$</t>
+          <t>1.32$</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="I20:K20"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
@@ -2651,12 +3021,28 @@
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
@@ -2669,10 +3055,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2712,16 +3098,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="16" t="inlineStr">
         <is>
-          <t>13.13$</t>
+          <t>8.23$</t>
         </is>
       </c>
       <c r="D2" s="16" t="inlineStr">
         <is>
-          <t>3.28$</t>
+          <t>1.65$</t>
         </is>
       </c>
     </row>
@@ -2732,223 +3118,223 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="16" t="inlineStr">
         <is>
-          <t>-3.35$</t>
+          <t>-3.27$</t>
         </is>
       </c>
       <c r="D3" s="16" t="inlineStr">
         <is>
-          <t>-0.67$</t>
+          <t>-0.55$</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>BNTX</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="16" t="inlineStr">
         <is>
-          <t>-1.59$</t>
+          <t>-5.15$</t>
         </is>
       </c>
       <c r="D4" s="16" t="inlineStr">
         <is>
-          <t>-0.53$</t>
+          <t>-5.15$</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="16" t="inlineStr">
         <is>
-          <t>-0.6$</t>
+          <t>-1.59$</t>
         </is>
       </c>
       <c r="D5" s="16" t="inlineStr">
         <is>
-          <t>-0.15$</t>
+          <t>-0.53$</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FB</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>-3.56$</t>
+          <t>-0.34$</t>
         </is>
       </c>
       <c r="D6" s="16" t="inlineStr">
         <is>
-          <t>-0.89$</t>
+          <t>-0.07$</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GOOG</t>
+          <t>FB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="16" t="inlineStr">
         <is>
-          <t>7.63$</t>
+          <t>-3.81$</t>
         </is>
       </c>
       <c r="D7" s="16" t="inlineStr">
         <is>
-          <t>2.54$</t>
+          <t>-0.63$</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>GOOG</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="16" t="inlineStr">
         <is>
-          <t>-0.4$</t>
+          <t>9.46$</t>
         </is>
       </c>
       <c r="D8" s="16" t="inlineStr">
         <is>
-          <t>-0.08$</t>
+          <t>2.37$</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JNJ</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="16" t="inlineStr">
         <is>
-          <t>4.68$</t>
+          <t>-0.08$</t>
         </is>
       </c>
       <c r="D9" s="16" t="inlineStr">
         <is>
-          <t>0.94$</t>
+          <t>-0.01$</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LIT</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C10" s="16" t="inlineStr">
         <is>
-          <t>-2.19$</t>
+          <t>7.86$</t>
         </is>
       </c>
       <c r="D10" s="16" t="inlineStr">
         <is>
-          <t>-2.19$</t>
+          <t>1.12$</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MRNA</t>
+          <t>LIT</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" s="16" t="inlineStr">
         <is>
-          <t>-3.86$</t>
+          <t>-2.19$</t>
         </is>
       </c>
       <c r="D11" s="16" t="inlineStr">
         <is>
-          <t>-0.96$</t>
+          <t>-2.19$</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>MRNA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="16" t="inlineStr">
         <is>
-          <t>3.34$</t>
+          <t>-2.78$</t>
         </is>
       </c>
       <c r="D12" s="16" t="inlineStr">
         <is>
-          <t>0.37$</t>
+          <t>-0.35$</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MU</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>2.96$</t>
+          <t>3.34$</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>0.99$</t>
+          <t>0.37$</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>NFLX</t>
+          <t>MU</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -2956,154 +3342,328 @@
       </c>
       <c r="C14" s="16" t="inlineStr">
         <is>
-          <t>-0.78$</t>
+          <t>2.96$</t>
         </is>
       </c>
       <c r="D14" s="16" t="inlineStr">
         <is>
-          <t>-0.26$</t>
+          <t>0.99$</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>NVAX</t>
+          <t>NFLX</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15" s="16" t="inlineStr">
         <is>
-          <t>-12.53$</t>
+          <t>-1.62$</t>
         </is>
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>-2.09$</t>
+          <t>-0.4$</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>NVAX</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="16" t="inlineStr">
         <is>
-          <t>0.36$</t>
+          <t>-20.31$</t>
         </is>
       </c>
       <c r="D16" s="16" t="inlineStr">
         <is>
-          <t>0.04$</t>
+          <t>-2.54$</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>NVDA</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C17" s="16" t="inlineStr">
         <is>
-          <t>-5.83$</t>
+          <t>3.94$</t>
         </is>
       </c>
       <c r="D17" s="16" t="inlineStr">
         <is>
-          <t>-1.94$</t>
+          <t>0.39$</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PHG</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" s="16" t="inlineStr">
         <is>
-          <t>-2.7$</t>
+          <t>-2.86$</t>
         </is>
       </c>
       <c r="D18" s="16" t="inlineStr">
         <is>
-          <t>-2.7$</t>
+          <t>-0.57$</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TSLA</t>
+          <t>PHG</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" s="16" t="inlineStr">
         <is>
-          <t>5.93$</t>
+          <t>-2.7$</t>
         </is>
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>1.98$</t>
+          <t>-2.7$</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>TSLA</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20" s="16" t="inlineStr">
         <is>
-          <t>-0.94$</t>
+          <t>8.89$</t>
         </is>
       </c>
       <c r="D20" s="16" t="inlineStr">
         <is>
-          <t>-0.94$</t>
+          <t>1.78$</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="16" t="inlineStr">
+        <is>
+          <t>-0.94$</t>
+        </is>
+      </c>
+      <c r="D21" s="16" t="inlineStr">
+        <is>
+          <t>-0.94$</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>VIR</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" s="16" t="inlineStr">
-        <is>
-          <t>-5.57$</t>
-        </is>
-      </c>
-      <c r="D21" s="16" t="inlineStr">
-        <is>
-          <t>-1.86$</t>
-        </is>
-      </c>
+      <c r="B22" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" s="16" t="inlineStr">
+        <is>
+          <t>-8.75$</t>
+        </is>
+      </c>
+      <c r="D22" s="16" t="inlineStr">
+        <is>
+          <t>-2.19$</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="16" t="n"/>
+      <c r="D23" s="16" t="n"/>
+    </row>
+    <row r="24">
+      <c r="C24" s="16" t="n"/>
+      <c r="D24" s="16" t="n"/>
+    </row>
+    <row r="25">
+      <c r="C25" s="16" t="n"/>
+      <c r="D25" s="16" t="n"/>
+    </row>
+    <row r="26">
+      <c r="C26" s="16" t="n"/>
+      <c r="D26" s="16" t="n"/>
+    </row>
+    <row r="27">
+      <c r="C27" s="16" t="n"/>
+      <c r="D27" s="16" t="n"/>
+    </row>
+    <row r="28">
+      <c r="C28" s="16" t="n"/>
+      <c r="D28" s="16" t="n"/>
+    </row>
+    <row r="29">
+      <c r="C29" s="16" t="n"/>
+      <c r="D29" s="16" t="n"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="16" t="n"/>
+      <c r="D30" s="16" t="n"/>
+    </row>
+    <row r="31">
+      <c r="C31" s="16" t="n"/>
+      <c r="D31" s="16" t="n"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="16" t="n"/>
+      <c r="D32" s="16" t="n"/>
+    </row>
+    <row r="33">
+      <c r="C33" s="16" t="n"/>
+      <c r="D33" s="16" t="n"/>
+    </row>
+    <row r="34">
+      <c r="C34" s="16" t="n"/>
+      <c r="D34" s="16" t="n"/>
+    </row>
+    <row r="35">
+      <c r="C35" s="16" t="n"/>
+      <c r="D35" s="16" t="n"/>
+    </row>
+    <row r="36">
+      <c r="C36" s="16" t="n"/>
+      <c r="D36" s="16" t="n"/>
+    </row>
+    <row r="37">
+      <c r="C37" s="16" t="n"/>
+      <c r="D37" s="16" t="n"/>
+    </row>
+    <row r="38">
+      <c r="C38" s="16" t="n"/>
+      <c r="D38" s="16" t="n"/>
+    </row>
+    <row r="39">
+      <c r="C39" s="16" t="n"/>
+      <c r="D39" s="16" t="n"/>
+    </row>
+    <row r="40">
+      <c r="C40" s="16" t="n"/>
+      <c r="D40" s="16" t="n"/>
+    </row>
+    <row r="41">
+      <c r="C41" s="16" t="n"/>
+      <c r="D41" s="16" t="n"/>
+    </row>
+    <row r="42">
+      <c r="C42" s="16" t="n"/>
+      <c r="D42" s="16" t="n"/>
+    </row>
+    <row r="43">
+      <c r="C43" s="16" t="n"/>
+      <c r="D43" s="16" t="n"/>
+    </row>
+    <row r="44">
+      <c r="C44" s="16" t="n"/>
+      <c r="D44" s="16" t="n"/>
+    </row>
+    <row r="45">
+      <c r="C45" s="16" t="n"/>
+      <c r="D45" s="16" t="n"/>
+    </row>
+    <row r="46">
+      <c r="C46" s="16" t="n"/>
+      <c r="D46" s="16" t="n"/>
+    </row>
+    <row r="47">
+      <c r="C47" s="16" t="n"/>
+      <c r="D47" s="16" t="n"/>
+    </row>
+    <row r="48">
+      <c r="C48" s="16" t="n"/>
+      <c r="D48" s="16" t="n"/>
+    </row>
+    <row r="49">
+      <c r="C49" s="16" t="n"/>
+      <c r="D49" s="16" t="n"/>
+    </row>
+    <row r="50">
+      <c r="C50" s="16" t="n"/>
+      <c r="D50" s="16" t="n"/>
+    </row>
+    <row r="51">
+      <c r="C51" s="16" t="n"/>
+      <c r="D51" s="16" t="n"/>
+    </row>
+    <row r="52">
+      <c r="C52" s="16" t="n"/>
+      <c r="D52" s="16" t="n"/>
+    </row>
+    <row r="53">
+      <c r="C53" s="16" t="n"/>
+      <c r="D53" s="16" t="n"/>
+    </row>
+    <row r="54">
+      <c r="C54" s="16" t="n"/>
+    </row>
+    <row r="55">
+      <c r="C55" s="16" t="n"/>
+    </row>
+    <row r="56">
+      <c r="C56" s="16" t="n"/>
+    </row>
+    <row r="57">
+      <c r="C57" s="16" t="n"/>
+    </row>
+    <row r="58">
+      <c r="C58" s="16" t="n"/>
+    </row>
+    <row r="59">
+      <c r="C59" s="16" t="n"/>
+    </row>
+    <row r="60">
+      <c r="C60" s="16" t="n"/>
+    </row>
+    <row r="61">
+      <c r="C61" s="16" t="n"/>
+    </row>
+    <row r="62">
+      <c r="C62" s="16" t="n"/>
+    </row>
+    <row r="63">
+      <c r="C63" s="16" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>